<commit_message>
commit A1 VERSION 0.9.8
</commit_message>
<xml_diff>
--- a/database_exel.xlsx
+++ b/database_exel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,61 +478,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ва</t>
+          <t>СОШ №6</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>06/09/2022</t>
+          <t>13/09/2022</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Питание, продукты</t>
+          <t>Покупка вещей</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>851.76</v>
+        <v>1256.832</v>
       </c>
       <c r="F2" t="n">
-        <v>65.4145</v>
+        <v>96</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>все круто</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Ден</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>БГМУ</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>06/09/2022</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Поездка в школу</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>58.604</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>класс</t>
+          <t>сраероаеоаеовк</t>
         </is>
       </c>
     </row>

</xml_diff>